<commit_message>
Cambios en archivo excel, reduccion zoom
</commit_message>
<xml_diff>
--- a/estadistica.xlsx
+++ b/estadistica.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Dropbox\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Dropbox\Workspace\Web\estadistica-paros\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -680,9 +680,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -752,21 +749,6 @@
     <xf numFmtId="0" fontId="1" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -793,6 +775,24 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4840,7 +4840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -4882,7 +4882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC998"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -5754,16 +5754,16 @@
     </row>
     <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="31" t="str">
+      <c r="B24" s="63" t="str">
         <f>"PREDICCIONES SEMANA "&amp;B25</f>
         <v>PREDICCIONES SEMANA 7</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="63"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -5787,25 +5787,25 @@
     </row>
     <row r="25" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="32">
+      <c r="B25" s="31">
         <v>7</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="36" t="s">
+      <c r="G25" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="36" t="s">
+      <c r="H25" s="35" t="s">
         <v>30</v>
       </c>
       <c r="L25" s="4"/>
@@ -5831,27 +5831,27 @@
       <c r="B26" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="37">
+      <c r="C26" s="36">
         <f>H4+I19</f>
         <v>1453</v>
       </c>
-      <c r="D26" s="38">
+      <c r="D26" s="37">
         <f>_xlfn.FORECAST.LINEAR(B25,C4:H4,C2:H2)</f>
         <v>1571</v>
       </c>
-      <c r="E26" s="39">
+      <c r="E26" s="38">
         <f>INT(_xlfn.FORECAST.ETS(B25,C4:H4,C2:H2))</f>
         <v>1627</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="39">
         <f>G4+'2015'!I19</f>
         <v>2211</v>
       </c>
-      <c r="G26" s="41">
+      <c r="G26" s="40">
         <f>INT(_xlfn.FORECAST.LINEAR(B25+1,'2015'!C4:H4,'2015'!C2:H2))</f>
         <v>2018</v>
       </c>
-      <c r="H26" s="41">
+      <c r="H26" s="40">
         <f>INT(_xlfn.FORECAST.ETS(B25+1,'2015'!C4:H4,'2015'!C2:H2))</f>
         <v>2167</v>
       </c>
@@ -5878,27 +5878,27 @@
       <c r="B27" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="42">
+      <c r="C27" s="41">
         <f>C26/UNIVERSO!$C$3</f>
         <v>0.28401094605160282</v>
       </c>
-      <c r="D27" s="42">
+      <c r="D27" s="41">
         <f>D26/UNIVERSO!$C$3</f>
         <v>0.30707584050039094</v>
       </c>
-      <c r="E27" s="42">
+      <c r="E27" s="41">
         <f>E26/UNIVERSO!$C$3</f>
         <v>0.31802189210320564</v>
       </c>
-      <c r="F27" s="43">
+      <c r="F27" s="42">
         <f>F26/UNIVERSO!$C$3</f>
         <v>0.43217357310398746</v>
       </c>
-      <c r="G27" s="43">
+      <c r="G27" s="42">
         <f>G26/UNIVERSO!$C$3</f>
         <v>0.39444878811571538</v>
       </c>
-      <c r="H27" s="43">
+      <c r="H27" s="42">
         <f>H26/UNIVERSO!$C$3</f>
         <v>0.42357310398749021</v>
       </c>
@@ -5925,27 +5925,27 @@
       <c r="B28" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="44">
+      <c r="C28" s="43">
         <f>C26-0.4*UNIVERSO!$C$3</f>
         <v>-593.40000000000009</v>
       </c>
-      <c r="D28" s="44">
+      <c r="D28" s="43">
         <f>D26-0.4*UNIVERSO!$C$3</f>
         <v>-475.40000000000009</v>
       </c>
-      <c r="E28" s="44">
+      <c r="E28" s="43">
         <f>E26-0.4*UNIVERSO!$C$3</f>
         <v>-419.40000000000009</v>
       </c>
-      <c r="F28" s="45">
+      <c r="F28" s="44">
         <f>F26-0.4*UNIVERSO!$C$3</f>
         <v>164.59999999999991</v>
       </c>
-      <c r="G28" s="45">
+      <c r="G28" s="44">
         <f>G26-0.4*UNIVERSO!$C$3</f>
         <v>-28.400000000000091</v>
       </c>
-      <c r="H28" s="45">
+      <c r="H28" s="44">
         <f>H26-0.4*UNIVERSO!$C$3</f>
         <v>120.59999999999991</v>
       </c>
@@ -5972,27 +5972,27 @@
       <c r="B29" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C29" s="45">
         <f>H7+I20</f>
         <v>373</v>
       </c>
-      <c r="D29" s="47">
+      <c r="D29" s="46">
         <f>INT(_xlfn.FORECAST.LINEAR(B25,C7:H7,C2:H2))</f>
         <v>570</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="38">
         <f>INT(_xlfn.FORECAST.ETS(B25,C7:H7,C2:H2))</f>
         <v>582</v>
       </c>
-      <c r="F29" s="48">
+      <c r="F29" s="47">
         <f>G7+'2015'!I20</f>
         <v>1075</v>
       </c>
-      <c r="G29" s="41">
+      <c r="G29" s="40">
         <f>INT(_xlfn.FORECAST.LINEAR(B25+1,'2015'!C7:H7,'2015'!C2:H2))</f>
         <v>852</v>
       </c>
-      <c r="H29" s="41">
+      <c r="H29" s="40">
         <f>INT(_xlfn.FORECAST.ETS(B25+1,'2015'!C7:H7,'2015'!C2:H2))</f>
         <v>865</v>
       </c>
@@ -6019,27 +6019,27 @@
       <c r="B30" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="46">
+      <c r="C30" s="45">
         <f>H8+I21</f>
         <v>1027</v>
       </c>
-      <c r="D30" s="47">
+      <c r="D30" s="46">
         <f>INT(_xlfn.FORECAST.LINEAR(B25,C8:H8,C2:H2))</f>
         <v>951</v>
       </c>
-      <c r="E30" s="39">
+      <c r="E30" s="38">
         <f>INT(_xlfn.FORECAST.ETS(B25,C8:H8,C2:H2))</f>
         <v>1068</v>
       </c>
-      <c r="F30" s="48">
+      <c r="F30" s="47">
         <f>G8+'2015'!I21</f>
         <v>1084</v>
       </c>
-      <c r="G30" s="41">
+      <c r="G30" s="40">
         <f>INT(_xlfn.FORECAST.LINEAR(B25+1,'2015'!C8:H8,'2015'!C2:H2))</f>
         <v>1095</v>
       </c>
-      <c r="H30" s="41">
+      <c r="H30" s="40">
         <f>INT(_xlfn.FORECAST.ETS(B25+1,'2015'!C8:H8,'2015'!C2:H2))</f>
         <v>1250</v>
       </c>
@@ -6066,27 +6066,27 @@
       <c r="B31" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="46">
+      <c r="C31" s="45">
         <f>C26-SUM(C29:C30)</f>
         <v>53</v>
       </c>
-      <c r="D31" s="46">
+      <c r="D31" s="45">
         <f t="shared" ref="D31:H31" si="9">D26-SUM(D29:D30)</f>
         <v>50</v>
       </c>
-      <c r="E31" s="46">
+      <c r="E31" s="45">
         <f t="shared" si="9"/>
         <v>-23</v>
       </c>
-      <c r="F31" s="48">
+      <c r="F31" s="47">
         <f t="shared" si="9"/>
         <v>52</v>
       </c>
-      <c r="G31" s="48">
+      <c r="G31" s="47">
         <f t="shared" si="9"/>
         <v>71</v>
       </c>
-      <c r="H31" s="48">
+      <c r="H31" s="47">
         <f t="shared" si="9"/>
         <v>52</v>
       </c>
@@ -6113,27 +6113,27 @@
       <c r="B32" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="46">
+      <c r="C32" s="45">
         <f>C29-C30</f>
         <v>-654</v>
       </c>
-      <c r="D32" s="46">
+      <c r="D32" s="45">
         <f t="shared" ref="D32:H32" si="10">D29-D30</f>
         <v>-381</v>
       </c>
-      <c r="E32" s="46">
+      <c r="E32" s="45">
         <f t="shared" si="10"/>
         <v>-486</v>
       </c>
-      <c r="F32" s="48">
+      <c r="F32" s="47">
         <f t="shared" si="10"/>
         <v>-9</v>
       </c>
-      <c r="G32" s="48">
+      <c r="G32" s="47">
         <f t="shared" si="10"/>
         <v>-243</v>
       </c>
-      <c r="H32" s="48">
+      <c r="H32" s="47">
         <f t="shared" si="10"/>
         <v>-385</v>
       </c>
@@ -6160,27 +6160,27 @@
       <c r="B33" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="49">
+      <c r="C33" s="48">
         <f>C32/C26</f>
         <v>-0.45010323468685476</v>
       </c>
-      <c r="D33" s="49">
+      <c r="D33" s="48">
         <f t="shared" ref="D33:H33" si="11">D32/D26</f>
         <v>-0.24252068746021643</v>
       </c>
-      <c r="E33" s="49">
+      <c r="E33" s="48">
         <f t="shared" si="11"/>
         <v>-0.29870928088506454</v>
       </c>
-      <c r="F33" s="50">
+      <c r="F33" s="49">
         <f t="shared" si="11"/>
         <v>-4.0705563093622792E-3</v>
       </c>
-      <c r="G33" s="50">
+      <c r="G33" s="49">
         <f t="shared" si="11"/>
         <v>-0.12041625371655104</v>
       </c>
-      <c r="H33" s="50">
+      <c r="H33" s="49">
         <f t="shared" si="11"/>
         <v>-0.17766497461928935</v>
       </c>
@@ -6207,27 +6207,27 @@
       <c r="B34" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="51">
+      <c r="C34" s="50">
         <f>C29/C26</f>
         <v>0.25671025464556091</v>
       </c>
-      <c r="D34" s="51">
+      <c r="D34" s="50">
         <f t="shared" ref="D34:H34" si="12">D29/D26</f>
         <v>0.36282622533418207</v>
       </c>
-      <c r="E34" s="51">
+      <c r="E34" s="50">
         <f t="shared" si="12"/>
         <v>0.35771358328211433</v>
       </c>
-      <c r="F34" s="52">
+      <c r="F34" s="51">
         <f t="shared" si="12"/>
         <v>0.48620533695160562</v>
       </c>
-      <c r="G34" s="52">
+      <c r="G34" s="51">
         <f t="shared" si="12"/>
         <v>0.42220019821605548</v>
       </c>
-      <c r="H34" s="52">
+      <c r="H34" s="51">
         <f t="shared" si="12"/>
         <v>0.39916935856022151</v>
       </c>
@@ -6254,27 +6254,27 @@
       <c r="B35" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="51">
+      <c r="C35" s="50">
         <f>C30/C26</f>
         <v>0.70681348933241572</v>
       </c>
-      <c r="D35" s="51">
+      <c r="D35" s="50">
         <f t="shared" ref="D35:H35" si="13">D30/D26</f>
         <v>0.60534691279439845</v>
       </c>
-      <c r="E35" s="51">
+      <c r="E35" s="50">
         <f t="shared" si="13"/>
         <v>0.65642286416717888</v>
       </c>
-      <c r="F35" s="52">
+      <c r="F35" s="51">
         <f t="shared" si="13"/>
         <v>0.49027589326096788</v>
       </c>
-      <c r="G35" s="52">
+      <c r="G35" s="51">
         <f t="shared" si="13"/>
         <v>0.54261645193260655</v>
       </c>
-      <c r="H35" s="52">
+      <c r="H35" s="51">
         <f t="shared" si="13"/>
         <v>0.57683433317951083</v>
       </c>
@@ -6301,27 +6301,27 @@
       <c r="B36" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="51">
+      <c r="C36" s="50">
         <f>C29/UNIVERSO!$C$3</f>
         <v>7.2908522283033614E-2</v>
       </c>
-      <c r="D36" s="51">
+      <c r="D36" s="50">
         <f>D29/UNIVERSO!$C$3</f>
         <v>0.11141516810007819</v>
       </c>
-      <c r="E36" s="51">
+      <c r="E36" s="50">
         <f>E29/UNIVERSO!$C$3</f>
         <v>0.11376075058639562</v>
       </c>
-      <c r="F36" s="52">
+      <c r="F36" s="51">
         <f>F29/UNIVERSO!$C$3</f>
         <v>0.2101250977326036</v>
       </c>
-      <c r="G36" s="52">
+      <c r="G36" s="51">
         <f>G29/UNIVERSO!$C$3</f>
         <v>0.16653635652853793</v>
       </c>
-      <c r="H36" s="52">
+      <c r="H36" s="51">
         <f>H29/UNIVERSO!$C$3</f>
         <v>0.16907740422204848</v>
       </c>
@@ -6348,27 +6348,27 @@
       <c r="B37" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="51">
+      <c r="C37" s="50">
         <f>C30/UNIVERSO!$C$3</f>
         <v>0.20074276778733385</v>
       </c>
-      <c r="D37" s="51">
+      <c r="D37" s="50">
         <f>D30/UNIVERSO!$C$3</f>
         <v>0.18588741204065676</v>
       </c>
-      <c r="E37" s="51">
+      <c r="E37" s="50">
         <f>E30/UNIVERSO!$C$3</f>
         <v>0.20875684128225175</v>
       </c>
-      <c r="F37" s="52">
+      <c r="F37" s="51">
         <f>F30/UNIVERSO!$C$3</f>
         <v>0.21188428459734168</v>
       </c>
-      <c r="G37" s="52">
+      <c r="G37" s="51">
         <f>G30/UNIVERSO!$C$3</f>
         <v>0.214034401876466</v>
       </c>
-      <c r="H37" s="52">
+      <c r="H37" s="51">
         <f>H30/UNIVERSO!$C$3</f>
         <v>0.24433150899139952</v>
       </c>
@@ -6392,30 +6392,30 @@
     </row>
     <row r="38" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="54" t="str">
+      <c r="C38" s="53" t="str">
         <f>IF(OR(MAX(C36:C37)&gt;=20.01%,C26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>SI</v>
       </c>
-      <c r="D38" s="54" t="str">
+      <c r="D38" s="53" t="str">
         <f>IF(OR(MAX(D36:D37)&gt;=20.01%,D26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>NO</v>
       </c>
-      <c r="E38" s="54" t="str">
+      <c r="E38" s="53" t="str">
         <f>IF(OR(MAX(E36:E37)&gt;=20.01%,E26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>SI</v>
       </c>
-      <c r="F38" s="54" t="str">
+      <c r="F38" s="53" t="str">
         <f>IF(OR(MAX(F36:F37)&gt;=20.01%,F26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>SI</v>
       </c>
-      <c r="G38" s="54" t="str">
+      <c r="G38" s="53" t="str">
         <f>IF(OR(MAX(G36:G37)&gt;=20.01%,G26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>SI</v>
       </c>
-      <c r="H38" s="54" t="str">
+      <c r="H38" s="53" t="str">
         <f>IF(OR(MAX(H36:H37)&gt;=20.01%,H26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>SI</v>
       </c>
@@ -6509,17 +6509,17 @@
     </row>
     <row r="41" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="55" t="s">
+      <c r="B41" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="57" t="s">
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="G41" s="58"/>
-      <c r="H41" s="59"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="68"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -6543,19 +6543,19 @@
     </row>
     <row r="42" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="60" t="s">
+      <c r="B42" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="62" t="s">
+      <c r="C42" s="55"/>
+      <c r="D42" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="E42" s="63"/>
-      <c r="F42" s="64" t="s">
+      <c r="E42" s="57"/>
+      <c r="F42" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="G42" s="65"/>
-      <c r="H42" s="66"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="60"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -35262,7 +35262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -35304,25 +35304,25 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="67">
+      <c r="B3" s="61">
         <v>2015</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="68" t="s">
+      <c r="H3" s="62" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="4"/>
@@ -35464,27 +35464,27 @@
         <v>6</v>
       </c>
       <c r="C9" s="16">
-        <f>C4-SUM(C7:C8)</f>
+        <f t="shared" ref="C9:H9" si="0">C4-SUM(C7:C8)</f>
         <v>21</v>
       </c>
       <c r="D9" s="16">
-        <f>D4-SUM(D7:D8)</f>
+        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="E9" s="16">
-        <f>E4-SUM(E7:E8)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="F9" s="16">
-        <f>F4-SUM(F7:F8)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="G9" s="16">
-        <f>G4-SUM(G7:G8)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="H9" s="16">
-        <f>H4-SUM(H7:H8)</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="I9" s="4"/>
@@ -35494,27 +35494,27 @@
         <v>12</v>
       </c>
       <c r="C10" s="16">
-        <f>C7-C8</f>
+        <f t="shared" ref="C10:H10" si="1">C7-C8</f>
         <v>521</v>
       </c>
       <c r="D10" s="16">
-        <f>D7-D8</f>
+        <f t="shared" si="1"/>
         <v>488</v>
       </c>
       <c r="E10" s="16">
-        <f>E7-E8</f>
+        <f t="shared" si="1"/>
         <v>446</v>
       </c>
       <c r="F10" s="16">
-        <f>F7-F8</f>
+        <f t="shared" si="1"/>
         <v>331</v>
       </c>
       <c r="G10" s="16">
-        <f>G7-G8</f>
+        <f t="shared" si="1"/>
         <v>226</v>
       </c>
       <c r="H10" s="16">
-        <f>H7-H8</f>
+        <f t="shared" si="1"/>
         <v>-158</v>
       </c>
       <c r="I10" s="4"/>
@@ -35524,27 +35524,27 @@
         <v>11</v>
       </c>
       <c r="C11" s="17">
-        <f>C10/C4</f>
+        <f t="shared" ref="C11:H11" si="2">C10/C4</f>
         <v>0.150839606253619</v>
       </c>
       <c r="D11" s="17">
-        <f>D10/D4</f>
+        <f t="shared" si="2"/>
         <v>0.17231638418079095</v>
       </c>
       <c r="E11" s="17">
-        <f>E10/E4</f>
+        <f t="shared" si="2"/>
         <v>0.16403089371092314</v>
       </c>
       <c r="F11" s="17">
-        <f>F10/F4</f>
+        <f t="shared" si="2"/>
         <v>0.1258076776890916</v>
       </c>
       <c r="G11" s="17">
-        <f>G10/G4</f>
+        <f t="shared" si="2"/>
         <v>8.8143525741029641E-2</v>
       </c>
       <c r="H11" s="17">
-        <f>H10/H4</f>
+        <f t="shared" si="2"/>
         <v>-6.4384678076609622E-2</v>
       </c>
       <c r="I11" s="4"/>
@@ -35554,27 +35554,27 @@
         <v>7</v>
       </c>
       <c r="C12" s="19">
-        <f>C7/C4</f>
+        <f t="shared" ref="C12:H12" si="3">C7/C4</f>
         <v>0.57237984944991316</v>
       </c>
       <c r="D12" s="19">
-        <f>D7/D4</f>
+        <f t="shared" si="3"/>
         <v>0.58015536723163841</v>
       </c>
       <c r="E12" s="19">
-        <f>E7/E4</f>
+        <f t="shared" si="3"/>
         <v>0.57410812798823097</v>
       </c>
       <c r="F12" s="19">
-        <f>F7/F4</f>
+        <f t="shared" si="3"/>
         <v>0.55340174838464462</v>
       </c>
       <c r="G12" s="19">
-        <f>G7/G4</f>
+        <f t="shared" si="3"/>
         <v>0.53432137285491421</v>
       </c>
       <c r="H12" s="19">
-        <f>H7/H4</f>
+        <f t="shared" si="3"/>
         <v>0.45680521597392015</v>
       </c>
       <c r="I12" s="4"/>
@@ -35584,27 +35584,27 @@
         <v>8</v>
       </c>
       <c r="C13" s="19">
-        <f>C8/C4</f>
+        <f t="shared" ref="C13:H13" si="4">C8/C4</f>
         <v>0.42154024319629413</v>
       </c>
       <c r="D13" s="19">
-        <f>D8/D4</f>
+        <f t="shared" si="4"/>
         <v>0.40783898305084748</v>
       </c>
       <c r="E13" s="19">
-        <f>E8/E4</f>
+        <f t="shared" si="4"/>
         <v>0.41007723427730786</v>
       </c>
       <c r="F13" s="19">
-        <f>F8/F4</f>
+        <f t="shared" si="4"/>
         <v>0.427594070695553</v>
       </c>
       <c r="G13" s="19">
-        <f>G8/G4</f>
+        <f t="shared" si="4"/>
         <v>0.44617784711388453</v>
       </c>
       <c r="H13" s="19">
-        <f>H8/H4</f>
+        <f t="shared" si="4"/>
         <v>0.52118989405052973</v>
       </c>
       <c r="I13" s="4"/>
@@ -35704,27 +35704,27 @@
         <v>24</v>
       </c>
       <c r="C18" s="25" t="str">
-        <f>C3</f>
+        <f t="shared" ref="C18:H18" si="5">C3</f>
         <v>26-27 MAYO</v>
       </c>
       <c r="D18" s="25" t="str">
-        <f>D3</f>
+        <f t="shared" si="5"/>
         <v>4-5 JUNIO</v>
       </c>
       <c r="E18" s="25" t="str">
-        <f>E3</f>
+        <f t="shared" si="5"/>
         <v>11-12 JUNIO</v>
       </c>
       <c r="F18" s="25" t="str">
-        <f>F3</f>
+        <f t="shared" si="5"/>
         <v>18-19 JUNIO</v>
       </c>
       <c r="G18" s="25" t="str">
-        <f>G3</f>
+        <f t="shared" si="5"/>
         <v>25-26 JUNIO</v>
       </c>
       <c r="H18" s="25" t="str">
-        <f>H3</f>
+        <f t="shared" si="5"/>
         <v>2-3 JULIO</v>
       </c>
       <c r="I18" s="25" t="s">
@@ -35771,23 +35771,23 @@
         <v>17</v>
       </c>
       <c r="D20" s="28">
-        <f>-(C7-D7)</f>
+        <f t="shared" ref="D20:H22" si="6">-(C7-D7)</f>
         <v>-334</v>
       </c>
       <c r="E20" s="28">
-        <f>-(D7-E7)</f>
+        <f t="shared" si="6"/>
         <v>-82</v>
       </c>
       <c r="F20" s="28">
-        <f>-(E7-F7)</f>
+        <f t="shared" si="6"/>
         <v>-105</v>
       </c>
       <c r="G20" s="28">
-        <f>-(F7-G7)</f>
+        <f t="shared" si="6"/>
         <v>-86</v>
       </c>
       <c r="H20" s="28">
-        <f>-(G7-H7)</f>
+        <f t="shared" si="6"/>
         <v>-249</v>
       </c>
       <c r="I20" s="28">
@@ -35803,23 +35803,23 @@
         <v>17</v>
       </c>
       <c r="D21" s="28">
-        <f>-(C8-D8)</f>
+        <f t="shared" si="6"/>
         <v>-301</v>
       </c>
       <c r="E21" s="28">
-        <f>-(D8-E8)</f>
+        <f t="shared" si="6"/>
         <v>-40</v>
       </c>
       <c r="F21" s="28">
-        <f>-(E8-F8)</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="G21" s="28">
-        <f>-(F8-G8)</f>
+        <f t="shared" si="6"/>
         <v>19</v>
       </c>
       <c r="H21" s="28">
-        <f>-(G8-H8)</f>
+        <f t="shared" si="6"/>
         <v>135</v>
       </c>
       <c r="I21" s="28">
@@ -35835,23 +35835,23 @@
         <v>17</v>
       </c>
       <c r="D22" s="28">
-        <f>-(C9-D9)</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="E22" s="28">
-        <f>-(D9-E9)</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="F22" s="28">
-        <f>-(E9-F9)</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="G22" s="28">
-        <f>-(F9-G9)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H22" s="28">
-        <f>-(G9-H9)</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="I22" s="28">
@@ -35873,7 +35873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se actualiza gitignore y se eliminan caracteres invalidos
</commit_message>
<xml_diff>
--- a/estadistica.xlsx
+++ b/estadistica.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,20 +12,17 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
-    <sheet name="UNIVERSO" sheetId="4" r:id="rId1"/>
+    <sheet name="COMPARACION" sheetId="3" r:id="rId1"/>
     <sheet name="2016" sheetId="1" r:id="rId2"/>
     <sheet name="2015" sheetId="2" r:id="rId3"/>
-    <sheet name="COMPARACIÓN" sheetId="3" r:id="rId4"/>
+    <sheet name="UNIVERSO" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
-  <si>
-    <t>AÑO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
   <si>
     <t>UNIVERSO</t>
   </si>
@@ -254,6 +251,18 @@
   </si>
   <si>
     <t>25-26 JULIO</t>
+  </si>
+  <si>
+    <t>ANO</t>
+  </si>
+  <si>
+    <t>DIFF SI-NO</t>
+  </si>
+  <si>
+    <t>SI % DE LOS VOTOS</t>
+  </si>
+  <si>
+    <t>SI % DEL UNIVERSO</t>
   </si>
 </sst>
 </file>
@@ -797,7 +806,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -820,1084 +829,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>VOTACIONES</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 2016</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2016'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SI</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2016'!$C$3:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>6 - 7 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13-14 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20-21 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24-28 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4-5 JULIO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2016'!$C$7:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2149</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1793</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1595</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1468</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1247</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>669</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-ECF1-43F7-ACF4-033335084E65}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2016'!$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>NO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2016'!$C$3:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>6 - 7 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13-14 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20-21 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24-28 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4-5 JULIO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2016'!$C$8:$H$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1445</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1094</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>994</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>971</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1120</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1097</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-ECF1-43F7-ACF4-033335084E65}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2016'!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL VOTOS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2016'!$C$3:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>6 - 7 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13-14 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20-21 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24-28 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4-5 JULIO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2016'!$C$4:$H$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3639</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2931</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2637</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2482</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2411</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1818</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-ECF1-43F7-ACF4-033335084E65}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="981500480"/>
-        <c:axId val="981519200"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="981500480"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="981519200"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="981519200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="981500480"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>VOTACIONES</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 2015</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2015'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SI</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2015'!$C$3:$H$3</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>26-27 MAYO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4-5 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11-12 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18-19 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25-26 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2-3 JULIO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2015'!$C$7:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1977</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1643</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1561</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1456</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1370</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1121</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A536-4555-A0B4-EC54D2BE0ED3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2015'!$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>NO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'2015'!$C$8:$H$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1456</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1155</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1115</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1125</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1144</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1279</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A536-4555-A0B4-EC54D2BE0ED3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2015'!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL VOTOS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'2015'!$C$4:$H$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3454</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2832</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2719</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2631</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2564</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2454</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A536-4555-A0B4-EC54D2BE0ED3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="981500480"/>
-        <c:axId val="981519200"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="981500480"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="981519200"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="981519200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="981500480"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2678,6 +1610,1083 @@
           <c:h val="0.39346122282623663"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>VOTACIONES</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 2016</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2016'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2016'!$C$3:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6 - 7 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13-14 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-21 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24-28 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4-5 JULIO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2016'!$C$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2149</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1595</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1468</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1247</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ECF1-43F7-ACF4-033335084E65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2016'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2016'!$C$3:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6 - 7 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13-14 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-21 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24-28 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4-5 JULIO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2016'!$C$8:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1094</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>971</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1097</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ECF1-43F7-ACF4-033335084E65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2016'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL VOTOS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2016'!$C$3:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6 - 7 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13-14 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-21 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24-28 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4-5 JULIO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2016'!$C$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3639</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2637</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2482</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1818</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-ECF1-43F7-ACF4-033335084E65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="981500480"/>
+        <c:axId val="981519200"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="981500480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981519200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="981519200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981500480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>VOTACIONES</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 2015</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015'!$C$3:$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>26-27 MAYO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4-5 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11-12 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18-19 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25-26 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2-3 JULIO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015'!$C$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1643</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1561</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1456</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1370</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A536-4555-A0B4-EC54D2BE0ED3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015'!$C$8:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1456</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1155</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1144</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1279</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A536-4555-A0B4-EC54D2BE0ED3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL VOTOS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015'!$C$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3454</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2832</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2719</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2631</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2564</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2454</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A536-4555-A0B4-EC54D2BE0ED3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="981500480"/>
+        <c:axId val="981519200"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="981500480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981519200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="981519200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981500480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4416,6 +4425,49 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>74507</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{426A13B2-1BB7-49C2-9B7D-BA098356EA68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -4455,7 +4507,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4476,49 +4528,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A3976DF-7774-4081-8BBE-50096DC974DB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>74507</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{426A13B2-1BB7-49C2-9B7D-BA098356EA68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4838,43 +4847,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
-        <v>2016</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5116</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>2015</v>
-      </c>
-      <c r="C4" s="3">
-        <v>4912</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4883,10 +4868,10 @@
   <dimension ref="A1:AC998"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.88671875" style="5" customWidth="1"/>
     <col min="2" max="2" width="26" style="5" bestFit="1" customWidth="1"/>
@@ -4936,7 +4921,7 @@
     <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -4966,7 +4951,7 @@
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4975,22 +4960,22 @@
         <v>2016</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
@@ -5000,13 +4985,13 @@
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
       <c r="AC3" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="12">
         <v>3639</v>
@@ -5034,13 +5019,13 @@
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
       <c r="AC4" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="14">
         <f>C4/UNIVERSO!$C$3</f>
@@ -5074,13 +5059,13 @@
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
       <c r="AC5" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="15">
         <f>C4-0.4*UNIVERSO!$C$3</f>
@@ -5115,13 +5100,13 @@
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
       <c r="AC6" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="16">
         <v>2149</v>
@@ -5150,13 +5135,13 @@
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
       <c r="AC7" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="16">
         <v>1445</v>
@@ -5185,13 +5170,13 @@
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="16">
         <v>45</v>
@@ -5223,7 +5208,7 @@
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="16" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C10" s="16">
         <f t="shared" ref="C10:H10" si="0">C7-C8</f>
@@ -5261,7 +5246,7 @@
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="17">
         <f t="shared" ref="C11:H11" si="1">C10/C4</f>
@@ -5299,7 +5284,7 @@
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="18" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C12" s="19">
         <f t="shared" ref="C12:H12" si="2">C7/C4</f>
@@ -5338,7 +5323,7 @@
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="19">
         <f t="shared" ref="C13:H13" si="3">C8/C4</f>
@@ -5377,7 +5362,7 @@
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="18" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C14" s="19">
         <f>C7/UNIVERSO!$C$3</f>
@@ -5416,7 +5401,7 @@
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="21">
         <f>C8/UNIVERSO!$C$3</f>
@@ -5455,7 +5440,7 @@
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="23" t="str">
         <f>IF(OR(MAX(C14:C15)&gt;=20.01%*UNIVERSO!$C$3,C4&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
@@ -5510,7 +5495,7 @@
     <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="25" t="str">
         <f>C3</f>
@@ -5537,7 +5522,7 @@
         <v>25-26 JULIO</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J18" s="27"/>
       <c r="T18" s="4"/>
@@ -5553,10 +5538,10 @@
     <row r="19" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="29">
         <f>D4-C4</f>
@@ -5596,10 +5581,10 @@
     <row r="20" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="29">
         <f>D7-C7</f>
@@ -5639,10 +5624,10 @@
     <row r="21" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="29">
         <f>D8-C8</f>
@@ -5682,10 +5667,10 @@
     <row r="22" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="29">
         <f>D9-C9</f>
@@ -5791,22 +5776,22 @@
         <v>7</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="35" t="s">
-        <v>34</v>
-      </c>
       <c r="H25" s="35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -5829,7 +5814,7 @@
     <row r="26" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="36">
         <f>H4+I19</f>
@@ -5876,7 +5861,7 @@
     <row r="27" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="41">
         <f>C26/UNIVERSO!$C$3</f>
@@ -5923,7 +5908,7 @@
     <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="43">
         <f>C26-0.4*UNIVERSO!$C$3</f>
@@ -5970,7 +5955,7 @@
     <row r="29" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" s="45">
         <f>H7+I20</f>
@@ -6017,7 +6002,7 @@
     <row r="30" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="45">
         <f>H8+I21</f>
@@ -6064,7 +6049,7 @@
     <row r="31" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" s="45">
         <f>C26-SUM(C29:C30)</f>
@@ -6111,7 +6096,7 @@
     <row r="32" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C32" s="45">
         <f>C29-C30</f>
@@ -6158,7 +6143,7 @@
     <row r="33" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C33" s="48">
         <f>C32/C26</f>
@@ -6205,7 +6190,7 @@
     <row r="34" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34" s="50">
         <f>C29/C26</f>
@@ -6252,7 +6237,7 @@
     <row r="35" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" s="50">
         <f>C30/C26</f>
@@ -6299,7 +6284,7 @@
     <row r="36" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" s="50">
         <f>C29/UNIVERSO!$C$3</f>
@@ -6346,7 +6331,7 @@
     <row r="37" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C37" s="50">
         <f>C30/UNIVERSO!$C$3</f>
@@ -6393,7 +6378,7 @@
     <row r="38" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" s="53" t="str">
         <f>IF(OR(MAX(C36:C37)&gt;=20.01%,C26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
@@ -6440,7 +6425,7 @@
     <row r="39" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="23" t="str">
         <f>IF(C38="NO","NO",IF(C36&gt;C37,"SI",IF(C37&gt;C36,"NO","EMPATE")))</f>
@@ -6510,13 +6495,13 @@
     <row r="41" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="65"/>
       <c r="D41" s="65"/>
       <c r="E41" s="65"/>
       <c r="F41" s="66" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G41" s="67"/>
       <c r="H41" s="68"/>
@@ -6544,15 +6529,15 @@
     <row r="42" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C42" s="55"/>
       <c r="D42" s="56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E42" s="57"/>
       <c r="F42" s="58" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G42" s="59"/>
       <c r="H42" s="60"/>
@@ -35263,10 +35248,10 @@
   <dimension ref="B1:I22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="22.88671875" style="5" bestFit="1" customWidth="1"/>
@@ -35281,7 +35266,7 @@
     <row r="1" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -35308,28 +35293,28 @@
         <v>2015</v>
       </c>
       <c r="C3" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="E3" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="F3" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="G3" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="H3" s="62" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" s="62" t="s">
-        <v>23</v>
       </c>
       <c r="I3" s="4"/>
     </row>
     <row r="4" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="13">
         <v>3454</v>
@@ -35353,7 +35338,7 @@
     </row>
     <row r="5" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="14">
         <f>C4/UNIVERSO!$C$4</f>
@@ -35383,7 +35368,7 @@
     </row>
     <row r="6" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="15">
         <f>C4-0.4*UNIVERSO!$C$4</f>
@@ -35413,7 +35398,7 @@
     </row>
     <row r="7" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="16">
         <v>1977</v>
@@ -35437,7 +35422,7 @@
     </row>
     <row r="8" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="16">
         <v>1456</v>
@@ -35461,7 +35446,7 @@
     </row>
     <row r="9" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="16">
         <f t="shared" ref="C9:H9" si="0">C4-SUM(C7:C8)</f>
@@ -35491,7 +35476,7 @@
     </row>
     <row r="10" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="16">
         <f t="shared" ref="C10:H10" si="1">C7-C8</f>
@@ -35521,7 +35506,7 @@
     </row>
     <row r="11" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="17">
         <f t="shared" ref="C11:H11" si="2">C10/C4</f>
@@ -35551,7 +35536,7 @@
     </row>
     <row r="12" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C12" s="19">
         <f t="shared" ref="C12:H12" si="3">C7/C4</f>
@@ -35581,7 +35566,7 @@
     </row>
     <row r="13" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="19">
         <f t="shared" ref="C13:H13" si="4">C8/C4</f>
@@ -35611,7 +35596,7 @@
     </row>
     <row r="14" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C14" s="19">
         <f>C7/UNIVERSO!$C$4</f>
@@ -35641,7 +35626,7 @@
     </row>
     <row r="15" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="19">
         <f>C8/UNIVERSO!$C$4</f>
@@ -35671,7 +35656,7 @@
     </row>
     <row r="16" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="23" t="str">
         <f>IF(OR(MAX(C14:C15)&gt;=20.01%*UNIVERSO!$C$4,C4&gt;=40%*UNIVERSO!$C$4),"SI","NO")</f>
@@ -35701,7 +35686,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="25" t="str">
         <f t="shared" ref="C18:H18" si="5">C3</f>
@@ -35728,15 +35713,15 @@
         <v>2-3 JULIO</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="28">
         <f>-(C4-D4)</f>
@@ -35765,10 +35750,10 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D20" s="28">
         <f t="shared" ref="D20:H22" si="6">-(C7-D7)</f>
@@ -35797,10 +35782,10 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D21" s="28">
         <f t="shared" si="6"/>
@@ -35829,10 +35814,10 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D22" s="28">
         <f t="shared" si="6"/>
@@ -35871,18 +35856,42 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5116</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>2015</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4912</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se eliminan caracteres restrictivos. Orden de hojas
</commit_message>
<xml_diff>
--- a/estadistica.xlsx
+++ b/estadistica.xlsx
@@ -12,9 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
-    <sheet name="COMPARACION" sheetId="3" r:id="rId1"/>
-    <sheet name="2016" sheetId="1" r:id="rId2"/>
-    <sheet name="2015" sheetId="2" r:id="rId3"/>
+    <sheet name="2016" sheetId="1" r:id="rId1"/>
+    <sheet name="2015" sheetId="2" r:id="rId2"/>
+    <sheet name="COMPARACION" sheetId="3" r:id="rId3"/>
     <sheet name="UNIVERSO" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -99,31 +99,10 @@
     <t>PROM</t>
   </si>
   <si>
-    <t>¿SE CUMPLE CUORUM?</t>
-  </si>
-  <si>
-    <t>PROM AÑO</t>
-  </si>
-  <si>
     <t>DIFF SOBRE QS</t>
   </si>
   <si>
     <t>24-28 JUNIO</t>
-  </si>
-  <si>
-    <t>FRC EXP AÑO P</t>
-  </si>
-  <si>
-    <t>PROM AÑO P</t>
-  </si>
-  <si>
-    <t>FRC EXP AÑO</t>
-  </si>
-  <si>
-    <t>FRC LIN AÑO</t>
-  </si>
-  <si>
-    <t>FRC LIN AÑO P</t>
   </si>
   <si>
     <r>
@@ -142,63 +121,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> FORECAST(TENDENCIA, PRONOSTICO EXCEL)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>LIN:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> APROXIMACIÓN LINEAL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>AÑO P:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> AÑO PASADO (2015)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>EXP:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> APROXIMACIÓN EXPONENCIAL</t>
     </r>
   </si>
   <si>
@@ -244,9 +166,6 @@
     <t>OTROS</t>
   </si>
   <si>
-    <t>¿GANA PARO?</t>
-  </si>
-  <si>
     <t>4-5 JULIO</t>
   </si>
   <si>
@@ -263,6 +182,87 @@
   </si>
   <si>
     <t>SI % DEL UNIVERSO</t>
+  </si>
+  <si>
+    <t>SE CUMPLE CUORUM?</t>
+  </si>
+  <si>
+    <t>PROM ANO</t>
+  </si>
+  <si>
+    <t>FRC LIN ANO</t>
+  </si>
+  <si>
+    <t>FRC EXP ANO</t>
+  </si>
+  <si>
+    <t>PROM ANO P</t>
+  </si>
+  <si>
+    <t>FRC LIN ANO P</t>
+  </si>
+  <si>
+    <t>FRC EXP ANO P</t>
+  </si>
+  <si>
+    <t>GANA PARO?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ANO P:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> ANO PASADO (2015)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>LIN:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> APROXIMACION LINEAL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>EXP:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> APROXIMACION EXPONENCIAL</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -692,18 +692,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -758,14 +746,8 @@
     <xf numFmtId="0" fontId="1" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -794,13 +776,25 @@
     <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -827,6 +821,1083 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>VOTACIONES</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 2016</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2016'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2016'!$C$3:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6 - 7 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13-14 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-21 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24-28 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4-5 JULIO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2016'!$C$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2149</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1595</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1468</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1247</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>669</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ECF1-43F7-ACF4-033335084E65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2016'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2016'!$C$3:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6 - 7 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13-14 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-21 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24-28 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4-5 JULIO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2016'!$C$8:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1094</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>971</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1097</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ECF1-43F7-ACF4-033335084E65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2016'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL VOTOS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2016'!$C$3:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6 - 7 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13-14 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20-21 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24-28 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4-5 JULIO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2016'!$C$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3639</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2931</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2637</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2482</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1818</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-ECF1-43F7-ACF4-033335084E65}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="981500480"/>
+        <c:axId val="981519200"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="981500480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981519200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="981519200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981500480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>VOTACIONES</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 2015</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015'!$B$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015'!$C$3:$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>26-27 MAYO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4-5 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11-12 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18-19 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25-26 JUNIO</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2-3 JULIO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015'!$C$7:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1977</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1643</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1561</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1456</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1370</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A536-4555-A0B4-EC54D2BE0ED3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015'!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NO</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015'!$C$8:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1456</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1155</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1144</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1279</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A536-4555-A0B4-EC54D2BE0ED3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TOTAL VOTOS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015'!$C$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3454</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2832</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2719</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2631</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2564</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2454</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A536-4555-A0B4-EC54D2BE0ED3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="981500480"/>
+        <c:axId val="981519200"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="981500480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981519200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="981519200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="981500480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1610,1083 +2681,6 @@
           <c:h val="0.39346122282623663"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>VOTACIONES</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 2016</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2016'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SI</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2016'!$C$3:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>6 - 7 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13-14 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20-21 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24-28 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4-5 JULIO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2016'!$C$7:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2149</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1793</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1595</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1468</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1247</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>669</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-ECF1-43F7-ACF4-033335084E65}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2016'!$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>NO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2016'!$C$3:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>6 - 7 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13-14 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20-21 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24-28 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4-5 JULIO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2016'!$C$8:$H$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1445</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1094</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>994</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>971</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1120</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1097</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-ECF1-43F7-ACF4-033335084E65}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2016'!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL VOTOS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2016'!$C$3:$G$3</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>6 - 7 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13-14 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20-21 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>24-28 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4-5 JULIO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2016'!$C$4:$H$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3639</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2931</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2637</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2482</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2411</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1818</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-ECF1-43F7-ACF4-033335084E65}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="981500480"/>
-        <c:axId val="981519200"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="981500480"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="981519200"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="981519200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="981500480"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>VOTACIONES</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 2015</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2015'!$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SI</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2015'!$C$3:$H$3</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>26-27 MAYO</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4-5 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11-12 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>18-19 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25-26 JUNIO</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2-3 JULIO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2015'!$C$7:$H$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1977</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1643</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1561</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1456</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1370</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1121</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A536-4555-A0B4-EC54D2BE0ED3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2015'!$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>NO</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'2015'!$C$8:$H$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1456</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1155</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1115</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1125</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1144</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1279</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A536-4555-A0B4-EC54D2BE0ED3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2015'!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TOTAL VOTOS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'2015'!$C$4:$H$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3454</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2832</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2719</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2631</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2564</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2454</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A536-4555-A0B4-EC54D2BE0ED3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="981500480"/>
-        <c:axId val="981519200"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="981500480"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="981519200"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="981519200"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="981500480"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4425,49 +4419,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>74507</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{426A13B2-1BB7-49C2-9B7D-BA098356EA68}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -4507,7 +4458,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4528,6 +4479,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A3976DF-7774-4081-8BBE-50096DC974DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>74507</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{426A13B2-1BB7-49C2-9B7D-BA098356EA68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4847,28 +4841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC998"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4951,7 +4927,7 @@
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4969,13 +4945,13 @@
         <v>14</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
@@ -4985,7 +4961,7 @@
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
       <c r="AC3" s="11" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5019,7 +4995,7 @@
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
       <c r="AC4" s="11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5059,13 +5035,13 @@
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
       <c r="AC5" s="11" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="15">
         <f>C4-0.4*UNIVERSO!$C$3</f>
@@ -5100,7 +5076,7 @@
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
       <c r="AC6" s="11" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5135,7 +5111,7 @@
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
       <c r="AC7" s="11" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5170,7 +5146,7 @@
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="11" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5208,7 +5184,7 @@
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="16" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C10" s="16">
         <f t="shared" ref="C10:H10" si="0">C7-C8</f>
@@ -5284,7 +5260,7 @@
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="18" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C12" s="19">
         <f t="shared" ref="C12:H12" si="2">C7/C4</f>
@@ -5362,7 +5338,7 @@
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="18" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C14" s="19">
         <f>C7/UNIVERSO!$C$3</f>
@@ -5440,7 +5416,7 @@
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="22" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C16" s="23" t="str">
         <f>IF(OR(MAX(C14:C15)&gt;=20.01%*UNIVERSO!$C$3,C4&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
@@ -5739,16 +5715,16 @@
     </row>
     <row r="24" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="63" t="str">
+      <c r="B24" s="57" t="str">
         <f>"PREDICCIONES SEMANA "&amp;B25</f>
         <v>PREDICCIONES SEMANA 7</v>
       </c>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
+      <c r="C24" s="57"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -5775,23 +5751,23 @@
       <c r="B25" s="31">
         <v>7</v>
       </c>
-      <c r="C25" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" s="35" t="s">
-        <v>29</v>
+      <c r="C25" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="65" t="s">
+        <v>48</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -5816,27 +5792,27 @@
       <c r="B26" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="36">
+      <c r="C26" s="32">
         <f>H4+I19</f>
         <v>1453</v>
       </c>
-      <c r="D26" s="37">
+      <c r="D26" s="33">
         <f>_xlfn.FORECAST.LINEAR(B25,C4:H4,C2:H2)</f>
         <v>1571</v>
       </c>
-      <c r="E26" s="38">
+      <c r="E26" s="34">
         <f>INT(_xlfn.FORECAST.ETS(B25,C4:H4,C2:H2))</f>
         <v>1627</v>
       </c>
-      <c r="F26" s="39">
+      <c r="F26" s="35">
         <f>G4+'2015'!I19</f>
         <v>2211</v>
       </c>
-      <c r="G26" s="40">
+      <c r="G26" s="36">
         <f>INT(_xlfn.FORECAST.LINEAR(B25+1,'2015'!C4:H4,'2015'!C2:H2))</f>
         <v>2018</v>
       </c>
-      <c r="H26" s="40">
+      <c r="H26" s="36">
         <f>INT(_xlfn.FORECAST.ETS(B25+1,'2015'!C4:H4,'2015'!C2:H2))</f>
         <v>2167</v>
       </c>
@@ -5863,27 +5839,27 @@
       <c r="B27" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="41">
+      <c r="C27" s="37">
         <f>C26/UNIVERSO!$C$3</f>
         <v>0.28401094605160282</v>
       </c>
-      <c r="D27" s="41">
+      <c r="D27" s="37">
         <f>D26/UNIVERSO!$C$3</f>
         <v>0.30707584050039094</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="37">
         <f>E26/UNIVERSO!$C$3</f>
         <v>0.31802189210320564</v>
       </c>
-      <c r="F27" s="42">
+      <c r="F27" s="38">
         <f>F26/UNIVERSO!$C$3</f>
         <v>0.43217357310398746</v>
       </c>
-      <c r="G27" s="42">
+      <c r="G27" s="38">
         <f>G26/UNIVERSO!$C$3</f>
         <v>0.39444878811571538</v>
       </c>
-      <c r="H27" s="42">
+      <c r="H27" s="38">
         <f>H26/UNIVERSO!$C$3</f>
         <v>0.42357310398749021</v>
       </c>
@@ -5908,29 +5884,29 @@
     <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="43">
+        <v>25</v>
+      </c>
+      <c r="C28" s="39">
         <f>C26-0.4*UNIVERSO!$C$3</f>
         <v>-593.40000000000009</v>
       </c>
-      <c r="D28" s="43">
+      <c r="D28" s="39">
         <f>D26-0.4*UNIVERSO!$C$3</f>
         <v>-475.40000000000009</v>
       </c>
-      <c r="E28" s="43">
+      <c r="E28" s="39">
         <f>E26-0.4*UNIVERSO!$C$3</f>
         <v>-419.40000000000009</v>
       </c>
-      <c r="F28" s="44">
+      <c r="F28" s="40">
         <f>F26-0.4*UNIVERSO!$C$3</f>
         <v>164.59999999999991</v>
       </c>
-      <c r="G28" s="44">
+      <c r="G28" s="40">
         <f>G26-0.4*UNIVERSO!$C$3</f>
         <v>-28.400000000000091</v>
       </c>
-      <c r="H28" s="44">
+      <c r="H28" s="40">
         <f>H26-0.4*UNIVERSO!$C$3</f>
         <v>120.59999999999991</v>
       </c>
@@ -5957,27 +5933,27 @@
       <c r="B29" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="45">
+      <c r="C29" s="41">
         <f>H7+I20</f>
         <v>373</v>
       </c>
-      <c r="D29" s="46">
+      <c r="D29" s="42">
         <f>INT(_xlfn.FORECAST.LINEAR(B25,C7:H7,C2:H2))</f>
         <v>570</v>
       </c>
-      <c r="E29" s="38">
+      <c r="E29" s="34">
         <f>INT(_xlfn.FORECAST.ETS(B25,C7:H7,C2:H2))</f>
         <v>582</v>
       </c>
-      <c r="F29" s="47">
+      <c r="F29" s="43">
         <f>G7+'2015'!I20</f>
         <v>1075</v>
       </c>
-      <c r="G29" s="40">
+      <c r="G29" s="36">
         <f>INT(_xlfn.FORECAST.LINEAR(B25+1,'2015'!C7:H7,'2015'!C2:H2))</f>
         <v>852</v>
       </c>
-      <c r="H29" s="40">
+      <c r="H29" s="36">
         <f>INT(_xlfn.FORECAST.ETS(B25+1,'2015'!C7:H7,'2015'!C2:H2))</f>
         <v>865</v>
       </c>
@@ -6004,27 +5980,27 @@
       <c r="B30" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="45">
+      <c r="C30" s="41">
         <f>H8+I21</f>
         <v>1027</v>
       </c>
-      <c r="D30" s="46">
+      <c r="D30" s="42">
         <f>INT(_xlfn.FORECAST.LINEAR(B25,C8:H8,C2:H2))</f>
         <v>951</v>
       </c>
-      <c r="E30" s="38">
+      <c r="E30" s="34">
         <f>INT(_xlfn.FORECAST.ETS(B25,C8:H8,C2:H2))</f>
         <v>1068</v>
       </c>
-      <c r="F30" s="47">
+      <c r="F30" s="43">
         <f>G8+'2015'!I21</f>
         <v>1084</v>
       </c>
-      <c r="G30" s="40">
+      <c r="G30" s="36">
         <f>INT(_xlfn.FORECAST.LINEAR(B25+1,'2015'!C8:H8,'2015'!C2:H2))</f>
         <v>1095</v>
       </c>
-      <c r="H30" s="40">
+      <c r="H30" s="36">
         <f>INT(_xlfn.FORECAST.ETS(B25+1,'2015'!C8:H8,'2015'!C2:H2))</f>
         <v>1250</v>
       </c>
@@ -6051,27 +6027,27 @@
       <c r="B31" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="45">
+      <c r="C31" s="41">
         <f>C26-SUM(C29:C30)</f>
         <v>53</v>
       </c>
-      <c r="D31" s="45">
+      <c r="D31" s="41">
         <f t="shared" ref="D31:H31" si="9">D26-SUM(D29:D30)</f>
         <v>50</v>
       </c>
-      <c r="E31" s="45">
+      <c r="E31" s="41">
         <f t="shared" si="9"/>
         <v>-23</v>
       </c>
-      <c r="F31" s="47">
+      <c r="F31" s="43">
         <f t="shared" si="9"/>
         <v>52</v>
       </c>
-      <c r="G31" s="47">
+      <c r="G31" s="43">
         <f t="shared" si="9"/>
         <v>71</v>
       </c>
-      <c r="H31" s="47">
+      <c r="H31" s="43">
         <f t="shared" si="9"/>
         <v>52</v>
       </c>
@@ -6098,27 +6074,27 @@
       <c r="B32" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="45">
+      <c r="C32" s="41">
         <f>C29-C30</f>
         <v>-654</v>
       </c>
-      <c r="D32" s="45">
+      <c r="D32" s="41">
         <f t="shared" ref="D32:H32" si="10">D29-D30</f>
         <v>-381</v>
       </c>
-      <c r="E32" s="45">
+      <c r="E32" s="41">
         <f t="shared" si="10"/>
         <v>-486</v>
       </c>
-      <c r="F32" s="47">
+      <c r="F32" s="43">
         <f t="shared" si="10"/>
         <v>-9</v>
       </c>
-      <c r="G32" s="47">
+      <c r="G32" s="43">
         <f t="shared" si="10"/>
         <v>-243</v>
       </c>
-      <c r="H32" s="47">
+      <c r="H32" s="43">
         <f t="shared" si="10"/>
         <v>-385</v>
       </c>
@@ -6145,27 +6121,27 @@
       <c r="B33" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="48">
+      <c r="C33" s="44">
         <f>C32/C26</f>
         <v>-0.45010323468685476</v>
       </c>
-      <c r="D33" s="48">
+      <c r="D33" s="44">
         <f t="shared" ref="D33:H33" si="11">D32/D26</f>
         <v>-0.24252068746021643</v>
       </c>
-      <c r="E33" s="48">
+      <c r="E33" s="44">
         <f t="shared" si="11"/>
         <v>-0.29870928088506454</v>
       </c>
-      <c r="F33" s="49">
+      <c r="F33" s="45">
         <f t="shared" si="11"/>
         <v>-4.0705563093622792E-3</v>
       </c>
-      <c r="G33" s="49">
+      <c r="G33" s="45">
         <f t="shared" si="11"/>
         <v>-0.12041625371655104</v>
       </c>
-      <c r="H33" s="49">
+      <c r="H33" s="45">
         <f t="shared" si="11"/>
         <v>-0.17766497461928935</v>
       </c>
@@ -6192,27 +6168,27 @@
       <c r="B34" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="50">
+      <c r="C34" s="46">
         <f>C29/C26</f>
         <v>0.25671025464556091</v>
       </c>
-      <c r="D34" s="50">
+      <c r="D34" s="46">
         <f t="shared" ref="D34:H34" si="12">D29/D26</f>
         <v>0.36282622533418207</v>
       </c>
-      <c r="E34" s="50">
+      <c r="E34" s="46">
         <f t="shared" si="12"/>
         <v>0.35771358328211433</v>
       </c>
-      <c r="F34" s="51">
+      <c r="F34" s="47">
         <f t="shared" si="12"/>
         <v>0.48620533695160562</v>
       </c>
-      <c r="G34" s="51">
+      <c r="G34" s="47">
         <f t="shared" si="12"/>
         <v>0.42220019821605548</v>
       </c>
-      <c r="H34" s="51">
+      <c r="H34" s="47">
         <f t="shared" si="12"/>
         <v>0.39916935856022151</v>
       </c>
@@ -6239,27 +6215,27 @@
       <c r="B35" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="50">
+      <c r="C35" s="46">
         <f>C30/C26</f>
         <v>0.70681348933241572</v>
       </c>
-      <c r="D35" s="50">
+      <c r="D35" s="46">
         <f t="shared" ref="D35:H35" si="13">D30/D26</f>
         <v>0.60534691279439845</v>
       </c>
-      <c r="E35" s="50">
+      <c r="E35" s="46">
         <f t="shared" si="13"/>
         <v>0.65642286416717888</v>
       </c>
-      <c r="F35" s="51">
+      <c r="F35" s="47">
         <f t="shared" si="13"/>
         <v>0.49027589326096788</v>
       </c>
-      <c r="G35" s="51">
+      <c r="G35" s="47">
         <f t="shared" si="13"/>
         <v>0.54261645193260655</v>
       </c>
-      <c r="H35" s="51">
+      <c r="H35" s="47">
         <f t="shared" si="13"/>
         <v>0.57683433317951083</v>
       </c>
@@ -6286,27 +6262,27 @@
       <c r="B36" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="50">
+      <c r="C36" s="46">
         <f>C29/UNIVERSO!$C$3</f>
         <v>7.2908522283033614E-2</v>
       </c>
-      <c r="D36" s="50">
+      <c r="D36" s="46">
         <f>D29/UNIVERSO!$C$3</f>
         <v>0.11141516810007819</v>
       </c>
-      <c r="E36" s="50">
+      <c r="E36" s="46">
         <f>E29/UNIVERSO!$C$3</f>
         <v>0.11376075058639562</v>
       </c>
-      <c r="F36" s="51">
+      <c r="F36" s="47">
         <f>F29/UNIVERSO!$C$3</f>
         <v>0.2101250977326036</v>
       </c>
-      <c r="G36" s="51">
+      <c r="G36" s="47">
         <f>G29/UNIVERSO!$C$3</f>
         <v>0.16653635652853793</v>
       </c>
-      <c r="H36" s="51">
+      <c r="H36" s="47">
         <f>H29/UNIVERSO!$C$3</f>
         <v>0.16907740422204848</v>
       </c>
@@ -6333,27 +6309,27 @@
       <c r="B37" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="50">
+      <c r="C37" s="46">
         <f>C30/UNIVERSO!$C$3</f>
         <v>0.20074276778733385</v>
       </c>
-      <c r="D37" s="50">
+      <c r="D37" s="46">
         <f>D30/UNIVERSO!$C$3</f>
         <v>0.18588741204065676</v>
       </c>
-      <c r="E37" s="50">
+      <c r="E37" s="46">
         <f>E30/UNIVERSO!$C$3</f>
         <v>0.20875684128225175</v>
       </c>
-      <c r="F37" s="51">
+      <c r="F37" s="47">
         <f>F30/UNIVERSO!$C$3</f>
         <v>0.21188428459734168</v>
       </c>
-      <c r="G37" s="51">
+      <c r="G37" s="47">
         <f>G30/UNIVERSO!$C$3</f>
         <v>0.214034401876466</v>
       </c>
-      <c r="H37" s="51">
+      <c r="H37" s="47">
         <f>H30/UNIVERSO!$C$3</f>
         <v>0.24433150899139952</v>
       </c>
@@ -6377,30 +6353,30 @@
     </row>
     <row r="38" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="53" t="str">
+      <c r="B38" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="49" t="str">
         <f>IF(OR(MAX(C36:C37)&gt;=20.01%,C26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>SI</v>
       </c>
-      <c r="D38" s="53" t="str">
+      <c r="D38" s="49" t="str">
         <f>IF(OR(MAX(D36:D37)&gt;=20.01%,D26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>NO</v>
       </c>
-      <c r="E38" s="53" t="str">
+      <c r="E38" s="49" t="str">
         <f>IF(OR(MAX(E36:E37)&gt;=20.01%,E26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>SI</v>
       </c>
-      <c r="F38" s="53" t="str">
+      <c r="F38" s="49" t="str">
         <f>IF(OR(MAX(F36:F37)&gt;=20.01%,F26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>SI</v>
       </c>
-      <c r="G38" s="53" t="str">
+      <c r="G38" s="49" t="str">
         <f>IF(OR(MAX(G36:G37)&gt;=20.01%,G26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>SI</v>
       </c>
-      <c r="H38" s="53" t="str">
+      <c r="H38" s="49" t="str">
         <f>IF(OR(MAX(H36:H37)&gt;=20.01%,H26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
         <v>SI</v>
       </c>
@@ -6425,7 +6401,7 @@
     <row r="39" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C39" s="23" t="str">
         <f>IF(C38="NO","NO",IF(C36&gt;C37,"SI",IF(C37&gt;C36,"NO","EMPATE")))</f>
@@ -6494,17 +6470,17 @@
     </row>
     <row r="41" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
-      <c r="B41" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="65"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="66" t="s">
-        <v>37</v>
-      </c>
-      <c r="G41" s="67"/>
-      <c r="H41" s="68"/>
+      <c r="B41" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="59"/>
+      <c r="F41" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="G41" s="60"/>
+      <c r="H41" s="61"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -6528,19 +6504,19 @@
     </row>
     <row r="42" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
-      <c r="B42" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" s="55"/>
-      <c r="D42" s="56" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" s="57"/>
-      <c r="F42" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="G42" s="59"/>
-      <c r="H42" s="60"/>
+      <c r="B42" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="50"/>
+      <c r="D42" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" s="51"/>
+      <c r="F42" s="52" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" s="53"/>
+      <c r="H42" s="54"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
@@ -35243,12 +35219,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -35289,25 +35265,25 @@
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="61">
+      <c r="B3" s="55">
         <v>2015</v>
       </c>
-      <c r="C3" s="62" t="s">
+      <c r="C3" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="62" t="s">
+      <c r="E3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="62" t="s">
+      <c r="F3" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="62" t="s">
+      <c r="G3" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="62" t="s">
+      <c r="H3" s="56" t="s">
         <v>22</v>
       </c>
       <c r="I3" s="4"/>
@@ -35368,7 +35344,7 @@
     </row>
     <row r="6" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="15">
         <f>C4-0.4*UNIVERSO!$C$4</f>
@@ -35536,7 +35512,7 @@
     </row>
     <row r="12" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C12" s="19">
         <f t="shared" ref="C12:H12" si="3">C7/C4</f>
@@ -35596,7 +35572,7 @@
     </row>
     <row r="14" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C14" s="19">
         <f>C7/UNIVERSO!$C$4</f>
@@ -35656,7 +35632,7 @@
     </row>
     <row r="16" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C16" s="23" t="str">
         <f>IF(OR(MAX(C14:C15)&gt;=20.01%*UNIVERSO!$C$4,C4&gt;=40%*UNIVERSO!$C$4),"SI","NO")</f>
@@ -35851,6 +35827,24 @@
     <ignoredError sqref="C3:H3" twoDigitTextYear="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -35869,7 +35863,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Se borran caracteres no validos
</commit_message>
<xml_diff>
--- a/estadistica.xlsx
+++ b/estadistica.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>UNIVERSO</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>DIFF SI-NO %</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DIFF SI-NO    </t>
   </si>
   <si>
     <t>6 - 7 JUNIO</t>
@@ -4837,7 +4834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC998"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -4891,7 +4888,7 @@
     <row r="2" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -4921,7 +4918,7 @@
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4930,22 +4927,22 @@
         <v>2016</v>
       </c>
       <c r="C3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="10" t="s">
         <v>34</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>35</v>
       </c>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
@@ -4955,7 +4952,7 @@
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
       <c r="AC3" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4989,7 +4986,7 @@
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
       <c r="AC4" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5029,13 +5026,13 @@
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
       <c r="AC5" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="15">
         <f>C4-0.4*UNIVERSO!$C$3</f>
@@ -5070,7 +5067,7 @@
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
       <c r="AC6" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5105,7 +5102,7 @@
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
       <c r="AC7" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5140,7 +5137,7 @@
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5178,7 +5175,7 @@
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="16">
         <f t="shared" ref="C10:H10" si="0">C7-C8</f>
@@ -5254,7 +5251,7 @@
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="19">
         <f t="shared" ref="C12:H12" si="2">C7/C4</f>
@@ -5332,7 +5329,7 @@
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="19">
         <f>C7/UNIVERSO!$C$3</f>
@@ -5410,7 +5407,7 @@
     <row r="16" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="23" t="str">
         <f>IF(OR(MAX(C14:C15)&gt;=20.01%*UNIVERSO!$C$3,C4&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
@@ -5465,7 +5462,7 @@
     <row r="18" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="25" t="str">
         <f>C3</f>
@@ -5492,7 +5489,7 @@
         <v>25-26 JULIO</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J18" s="27"/>
       <c r="T18" s="4"/>
@@ -5511,7 +5508,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="29">
         <f>D4-C4</f>
@@ -5554,7 +5551,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="29">
         <f>D7-C7</f>
@@ -5597,7 +5594,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="29">
         <f>D8-C8</f>
@@ -5640,7 +5637,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="29">
         <f>D9-C9</f>
@@ -5746,22 +5743,22 @@
         <v>7</v>
       </c>
       <c r="C25" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="57" t="s">
+      <c r="E25" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="57" t="s">
+      <c r="F25" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="59" t="s">
+      <c r="G25" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="60" t="s">
+      <c r="H25" s="60" t="s">
         <v>45</v>
-      </c>
-      <c r="H25" s="60" t="s">
-        <v>46</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
@@ -5878,7 +5875,7 @@
     <row r="28" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="39">
         <f>C26-0.4*UNIVERSO!$C$3</f>
@@ -6066,7 +6063,7 @@
     <row r="32" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" s="41">
         <f>C29-C30</f>
@@ -6160,7 +6157,7 @@
     <row r="34" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="46">
         <f>C29/C26</f>
@@ -6254,7 +6251,7 @@
     <row r="36" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="46">
         <f>C29/UNIVERSO!$C$3</f>
@@ -6348,7 +6345,7 @@
     <row r="38" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" s="49" t="str">
         <f>IF(OR(MAX(C36:C37)&gt;=20.01%,C26&gt;=40%*UNIVERSO!$C$3),"SI","NO")</f>
@@ -6395,7 +6392,7 @@
     <row r="39" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" s="23" t="str">
         <f>IF(C38="NO","NO",IF(C36&gt;C37,"SI",IF(C37&gt;C36,"NO","EMPATE")))</f>
@@ -6465,13 +6462,13 @@
     <row r="41" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C41" s="64"/>
       <c r="D41" s="64"/>
       <c r="E41" s="64"/>
       <c r="F41" s="65" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G41" s="65"/>
       <c r="H41" s="66"/>
@@ -6499,15 +6496,15 @@
     <row r="42" spans="1:28" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" s="50"/>
       <c r="D42" s="51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E42" s="51"/>
       <c r="F42" s="52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G42" s="53"/>
       <c r="H42" s="54"/>
@@ -35217,8 +35214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -35236,7 +35233,7 @@
     <row r="1" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="6">
         <v>1</v>
@@ -35263,22 +35260,22 @@
         <v>2015</v>
       </c>
       <c r="C3" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="E3" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="F3" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="G3" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="H3" s="56" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" s="56" t="s">
-        <v>20</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -35338,7 +35335,7 @@
     </row>
     <row r="6" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="15">
         <f>C4-0.4*UNIVERSO!$C$4</f>
@@ -35446,7 +35443,7 @@
     </row>
     <row r="10" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C10" s="16">
         <f t="shared" ref="C10:H10" si="1">C7-C8</f>
@@ -35506,7 +35503,7 @@
     </row>
     <row r="12" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="19">
         <f t="shared" ref="C12:H12" si="3">C7/C4</f>
@@ -35566,7 +35563,7 @@
     </row>
     <row r="14" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="19">
         <f>C7/UNIVERSO!$C$4</f>
@@ -35626,7 +35623,7 @@
     </row>
     <row r="16" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="23" t="str">
         <f>IF(OR(MAX(C14:C15)&gt;=20.01%*UNIVERSO!$C$4,C4&gt;=40%*UNIVERSO!$C$4),"SI","NO")</f>
@@ -35656,7 +35653,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18" s="25" t="str">
         <f t="shared" ref="C18:H18" si="5">C3</f>
@@ -35683,7 +35680,7 @@
         <v>2-3 JULIO</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -35691,7 +35688,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="28">
         <f>-(C4-D4)</f>
@@ -35723,7 +35720,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="28">
         <f t="shared" ref="D20:H22" si="6">-(C7-D7)</f>
@@ -35755,7 +35752,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="28">
         <f t="shared" si="6"/>
@@ -35787,7 +35784,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="28">
         <f t="shared" si="6"/>
@@ -35857,7 +35854,7 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>

</xml_diff>